<commit_message>
fixed up total rec landings
</commit_message>
<xml_diff>
--- a/calfish_paper/tables/TableS3_other_datasets.xlsx
+++ b/calfish_paper/tables/TableS3_other_datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_landings_data/calfish_paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3181AF2-1E9A-F14A-BD2B-6D1850239090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C8714-D912-324B-AE93-8B265C0E66F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11040" yWindow="500" windowWidth="24800" windowHeight="20200" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="A1:D29"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>